<commit_message>
feat: implement authentication system with admin features
</commit_message>
<xml_diff>
--- a/public/pt_cleanedrecords.xlsx
+++ b/public/pt_cleanedrecords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\react-dashboard\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PT Projects\power-pipeline-dashboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5E55A7-5D8C-4CBF-B86E-4462BB93F330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE763EF-0DBF-4389-876A-2EEDBC62DD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{816DE86C-1293-4951-B1D8-131009567FC4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{816DE86C-1293-4951-B1D8-131009567FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="236">
   <si>
     <t>G</t>
   </si>
@@ -836,6 +836,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>PT</t>
   </si>
 </sst>
 </file>
@@ -2646,9 +2649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D5C93E-8E3B-466C-9E27-0F42C994458C}">
   <dimension ref="B1:AT50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.36328125" defaultRowHeight="16" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -6174,7 +6177,7 @@
     </row>
     <row r="34" spans="2:46" ht="34.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B34" s="37" t="s">
-        <v>57</v>
+        <v>235</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>58</v>
@@ -6214,7 +6217,7 @@
       </c>
       <c r="Q34" s="11"/>
       <c r="R34" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="S34" s="11" t="s">
         <v>171</v>
@@ -6292,7 +6295,7 @@
     </row>
     <row r="35" spans="2:46" ht="34.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B35" s="37" t="s">
-        <v>57</v>
+        <v>235</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>58</v>

</xml_diff>